<commit_message>
updating and adding file
</commit_message>
<xml_diff>
--- a/data/flights_EDA.xlsx
+++ b/data/flights_EDA.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13757" uniqueCount="4458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13757" uniqueCount="4456">
   <si>
     <t>NtsbNo</t>
   </si>
@@ -91,7 +91,7 @@
     <t>Region</t>
   </si>
   <si>
-    <t>NewCol</t>
+    <t>SecondaryCause</t>
   </si>
   <si>
     <t>ANC08MA038</t>
@@ -13345,31 +13345,28 @@
     <t>Pacific</t>
   </si>
   <si>
-    <t>Maintenance Issue</t>
-  </si>
-  <si>
-    <t>Runway</t>
-  </si>
-  <si>
-    <t>Lighting/Visibility</t>
-  </si>
-  <si>
-    <t>Object/Animal</t>
-  </si>
-  <si>
-    <t>Failure</t>
-  </si>
-  <si>
-    <t>Incorrect use/operation</t>
+    <t>Air_Maintenance Issue</t>
+  </si>
+  <si>
+    <t>Env_Runway</t>
+  </si>
+  <si>
+    <t>Env_Lighting/Visibility</t>
+  </si>
+  <si>
+    <t>Env_Object/Animal</t>
+  </si>
+  <si>
+    <t>Air_Failure</t>
+  </si>
+  <si>
+    <t>Aircraft Oper/Perf</t>
   </si>
   <si>
     <t>Pilot</t>
   </si>
   <si>
-    <t>Wind/Weather</t>
-  </si>
-  <si>
-    <t>Capability exceeded</t>
+    <t>Env_Wind/Weather</t>
   </si>
   <si>
     <t>Crew</t>
@@ -13378,13 +13375,13 @@
     <t>Env_Other</t>
   </si>
   <si>
-    <t>Damaged Part</t>
+    <t>Air_Damaged Part</t>
   </si>
   <si>
     <t>Not Determined</t>
   </si>
   <si>
-    <t>Turbulence</t>
+    <t>Env_Turbulence</t>
   </si>
   <si>
     <t>Air_Other</t>
@@ -13399,16 +13396,13 @@
     <t>Per_Other</t>
   </si>
   <si>
-    <t>Fluids</t>
-  </si>
-  <si>
     <t>Airport/Airline Personnel</t>
   </si>
   <si>
     <t>Ground Crew</t>
   </si>
   <si>
-    <t>Equipment</t>
+    <t>Env_Equipment</t>
   </si>
 </sst>
 </file>
@@ -14539,7 +14533,7 @@
         <v>4429</v>
       </c>
       <c r="Z10" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="11" spans="1:26">
@@ -14770,7 +14764,7 @@
         <v>4429</v>
       </c>
       <c r="Z13" t="s">
-        <v>4444</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="14" spans="1:26">
@@ -15155,7 +15149,7 @@
         <v>4429</v>
       </c>
       <c r="Z18" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="19" spans="1:26">
@@ -15309,7 +15303,7 @@
         <v>4429</v>
       </c>
       <c r="Z20" t="s">
-        <v>4444</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="21" spans="1:26">
@@ -15386,7 +15380,7 @@
         <v>4429</v>
       </c>
       <c r="Z21" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="22" spans="1:26">
@@ -15463,7 +15457,7 @@
         <v>4429</v>
       </c>
       <c r="Z22" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="23" spans="1:26">
@@ -15694,7 +15688,7 @@
         <v>4429</v>
       </c>
       <c r="Z25" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="26" spans="1:26">
@@ -15925,7 +15919,7 @@
         <v>4429</v>
       </c>
       <c r="Z28" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="29" spans="1:26">
@@ -16076,7 +16070,7 @@
         <v>4429</v>
       </c>
       <c r="Z30" t="s">
-        <v>4446</v>
+        <v>4445</v>
       </c>
     </row>
     <row r="31" spans="1:26">
@@ -16153,7 +16147,7 @@
         <v>4429</v>
       </c>
       <c r="Z31" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="32" spans="1:26">
@@ -16384,7 +16378,7 @@
         <v>4429</v>
       </c>
       <c r="Z34" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="35" spans="1:26">
@@ -16461,7 +16455,7 @@
         <v>4429</v>
       </c>
       <c r="Z35" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="36" spans="1:26">
@@ -16538,7 +16532,7 @@
         <v>4429</v>
       </c>
       <c r="Z36" t="s">
-        <v>4447</v>
+        <v>4446</v>
       </c>
     </row>
     <row r="37" spans="1:26">
@@ -16692,7 +16686,7 @@
         <v>4429</v>
       </c>
       <c r="Z38" t="s">
-        <v>4448</v>
+        <v>4447</v>
       </c>
     </row>
     <row r="39" spans="1:26">
@@ -16769,7 +16763,7 @@
         <v>4429</v>
       </c>
       <c r="Z39" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="40" spans="1:26">
@@ -16843,7 +16837,7 @@
         <v>4429</v>
       </c>
       <c r="Z40" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="41" spans="1:26">
@@ -16920,7 +16914,7 @@
         <v>4429</v>
       </c>
       <c r="Z41" t="s">
-        <v>4444</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="42" spans="1:26">
@@ -16997,7 +16991,7 @@
         <v>4429</v>
       </c>
       <c r="Z42" t="s">
-        <v>4444</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="43" spans="1:26">
@@ -17074,7 +17068,7 @@
         <v>4429</v>
       </c>
       <c r="Z43" t="s">
-        <v>4447</v>
+        <v>4446</v>
       </c>
     </row>
     <row r="44" spans="1:26">
@@ -17151,7 +17145,7 @@
         <v>4429</v>
       </c>
       <c r="Z44" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="45" spans="1:26">
@@ -17382,7 +17376,7 @@
         <v>4429</v>
       </c>
       <c r="Z47" t="s">
-        <v>4448</v>
+        <v>4447</v>
       </c>
     </row>
     <row r="48" spans="1:26">
@@ -17456,7 +17450,7 @@
         <v>4429</v>
       </c>
       <c r="Z48" t="s">
-        <v>4448</v>
+        <v>4447</v>
       </c>
     </row>
     <row r="49" spans="1:26">
@@ -17533,7 +17527,7 @@
         <v>4429</v>
       </c>
       <c r="Z49" t="s">
-        <v>4444</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="50" spans="1:26">
@@ -17995,7 +17989,7 @@
         <v>4429</v>
       </c>
       <c r="Z55" t="s">
-        <v>4447</v>
+        <v>4446</v>
       </c>
     </row>
     <row r="56" spans="1:26">
@@ -18072,7 +18066,7 @@
         <v>4429</v>
       </c>
       <c r="Z56" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="57" spans="1:26">
@@ -18303,7 +18297,7 @@
         <v>4429</v>
       </c>
       <c r="Z59" t="s">
-        <v>4446</v>
+        <v>4445</v>
       </c>
     </row>
     <row r="60" spans="1:26">
@@ -18380,7 +18374,7 @@
         <v>4429</v>
       </c>
       <c r="Z60" t="s">
-        <v>4447</v>
+        <v>4446</v>
       </c>
     </row>
     <row r="61" spans="1:26">
@@ -18534,7 +18528,7 @@
         <v>4429</v>
       </c>
       <c r="Z62" t="s">
-        <v>4450</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="63" spans="1:26">
@@ -18688,7 +18682,7 @@
         <v>4429</v>
       </c>
       <c r="Z64" t="s">
-        <v>4450</v>
+        <v>4449</v>
       </c>
     </row>
     <row r="65" spans="1:26">
@@ -19378,7 +19372,7 @@
         <v>4429</v>
       </c>
       <c r="Z73" t="s">
-        <v>4446</v>
+        <v>4445</v>
       </c>
     </row>
     <row r="74" spans="1:26">
@@ -20068,7 +20062,7 @@
         <v>4429</v>
       </c>
       <c r="Z82" t="s">
-        <v>4447</v>
+        <v>4446</v>
       </c>
     </row>
     <row r="83" spans="1:26">
@@ -20222,7 +20216,7 @@
         <v>4429</v>
       </c>
       <c r="Z84" t="s">
-        <v>4451</v>
+        <v>4450</v>
       </c>
     </row>
     <row r="85" spans="1:26">
@@ -20530,7 +20524,7 @@
         <v>4429</v>
       </c>
       <c r="Z88" t="s">
-        <v>4447</v>
+        <v>4446</v>
       </c>
     </row>
     <row r="89" spans="1:26">
@@ -20684,7 +20678,7 @@
         <v>4429</v>
       </c>
       <c r="Z90" t="s">
-        <v>4444</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="91" spans="1:26">
@@ -20835,7 +20829,7 @@
         <v>4429</v>
       </c>
       <c r="Z92" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="93" spans="1:26">
@@ -21140,7 +21134,7 @@
         <v>4429</v>
       </c>
       <c r="Z96" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="97" spans="1:26">
@@ -21371,7 +21365,7 @@
         <v>4429</v>
       </c>
       <c r="Z99" t="s">
-        <v>4452</v>
+        <v>4451</v>
       </c>
     </row>
     <row r="100" spans="1:26">
@@ -21599,7 +21593,7 @@
         <v>4429</v>
       </c>
       <c r="Z102" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="103" spans="1:26">
@@ -21904,7 +21898,7 @@
         <v>4429</v>
       </c>
       <c r="Z106" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="107" spans="1:26">
@@ -21981,7 +21975,7 @@
         <v>4429</v>
       </c>
       <c r="Z107" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="108" spans="1:26">
@@ -22058,7 +22052,7 @@
         <v>4429</v>
       </c>
       <c r="Z108" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="109" spans="1:26">
@@ -22976,7 +22970,7 @@
         <v>4429</v>
       </c>
       <c r="Z120" t="s">
-        <v>4448</v>
+        <v>4447</v>
       </c>
     </row>
     <row r="121" spans="1:26">
@@ -23666,7 +23660,7 @@
         <v>4429</v>
       </c>
       <c r="Z129" t="s">
-        <v>4448</v>
+        <v>4447</v>
       </c>
     </row>
     <row r="130" spans="1:26">
@@ -23743,7 +23737,7 @@
         <v>4429</v>
       </c>
       <c r="Z130" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="131" spans="1:26">
@@ -24590,7 +24584,7 @@
         <v>4429</v>
       </c>
       <c r="Z141" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="142" spans="1:26">
@@ -24667,7 +24661,7 @@
         <v>4429</v>
       </c>
       <c r="Z142" t="s">
-        <v>4450</v>
+        <v>4449</v>
       </c>
     </row>
     <row r="143" spans="1:26">
@@ -25123,7 +25117,7 @@
         <v>4429</v>
       </c>
       <c r="Z148" t="s">
-        <v>4448</v>
+        <v>4447</v>
       </c>
     </row>
     <row r="149" spans="1:26">
@@ -25508,7 +25502,7 @@
         <v>4429</v>
       </c>
       <c r="Z153" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="154" spans="1:26">
@@ -25585,7 +25579,7 @@
         <v>4429</v>
       </c>
       <c r="Z154" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="155" spans="1:26">
@@ -25739,7 +25733,7 @@
         <v>4429</v>
       </c>
       <c r="Z156" t="s">
-        <v>4450</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="157" spans="1:26">
@@ -25893,7 +25887,7 @@
         <v>4429</v>
       </c>
       <c r="Z158" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="159" spans="1:26">
@@ -26124,7 +26118,7 @@
         <v>4429</v>
       </c>
       <c r="Z161" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="162" spans="1:26">
@@ -26201,7 +26195,7 @@
         <v>4429</v>
       </c>
       <c r="Z162" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="163" spans="1:26">
@@ -26278,7 +26272,7 @@
         <v>4429</v>
       </c>
       <c r="Z163" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="164" spans="1:26">
@@ -26432,7 +26426,7 @@
         <v>4429</v>
       </c>
       <c r="Z165" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="166" spans="1:26">
@@ -26814,7 +26808,7 @@
         <v>4429</v>
       </c>
       <c r="Z170" t="s">
-        <v>4448</v>
+        <v>4447</v>
       </c>
     </row>
     <row r="171" spans="1:26">
@@ -26891,7 +26885,7 @@
         <v>4429</v>
       </c>
       <c r="Z171" t="s">
-        <v>4447</v>
+        <v>4446</v>
       </c>
     </row>
     <row r="172" spans="1:26">
@@ -27045,7 +27039,7 @@
         <v>4429</v>
       </c>
       <c r="Z173" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="174" spans="1:26">
@@ -27504,7 +27498,7 @@
         <v>4429</v>
       </c>
       <c r="Z179" t="s">
-        <v>4447</v>
+        <v>4446</v>
       </c>
     </row>
     <row r="180" spans="1:26">
@@ -28194,7 +28188,7 @@
         <v>4429</v>
       </c>
       <c r="Z188" t="s">
-        <v>4453</v>
+        <v>4452</v>
       </c>
     </row>
     <row r="189" spans="1:26">
@@ -28348,7 +28342,7 @@
         <v>4429</v>
       </c>
       <c r="Z190" t="s">
-        <v>4454</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="191" spans="1:26">
@@ -28807,7 +28801,7 @@
         <v>4429</v>
       </c>
       <c r="Z196" t="s">
-        <v>4450</v>
+        <v>4449</v>
       </c>
     </row>
     <row r="197" spans="1:26">
@@ -28881,7 +28875,7 @@
         <v>4429</v>
       </c>
       <c r="Z197" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="198" spans="1:26">
@@ -28955,7 +28949,7 @@
         <v>4429</v>
       </c>
       <c r="Z198" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="199" spans="1:26">
@@ -29029,7 +29023,7 @@
         <v>4429</v>
       </c>
       <c r="Z199" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="200" spans="1:26">
@@ -29180,7 +29174,7 @@
         <v>4429</v>
       </c>
       <c r="Z201" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="202" spans="1:26">
@@ -29334,7 +29328,7 @@
         <v>4429</v>
       </c>
       <c r="Z203" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="204" spans="1:26">
@@ -29485,7 +29479,7 @@
         <v>4429</v>
       </c>
       <c r="Z205" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="206" spans="1:26">
@@ -29562,7 +29556,7 @@
         <v>4429</v>
       </c>
       <c r="Z206" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="207" spans="1:26">
@@ -29639,7 +29633,7 @@
         <v>4430</v>
       </c>
       <c r="Z207" t="s">
-        <v>4455</v>
+        <v>4453</v>
       </c>
     </row>
     <row r="208" spans="1:26">
@@ -29947,7 +29941,7 @@
         <v>4430</v>
       </c>
       <c r="Z211" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="212" spans="1:26">
@@ -30024,7 +30018,7 @@
         <v>4430</v>
       </c>
       <c r="Z212" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="213" spans="1:26">
@@ -30249,7 +30243,7 @@
         <v>4430</v>
       </c>
       <c r="Z215" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="216" spans="1:26">
@@ -30400,7 +30394,7 @@
         <v>4430</v>
       </c>
       <c r="Z217" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="218" spans="1:26">
@@ -30554,7 +30548,7 @@
         <v>4430</v>
       </c>
       <c r="Z219" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="220" spans="1:26">
@@ -30708,7 +30702,7 @@
         <v>4429</v>
       </c>
       <c r="Z221" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="222" spans="1:26">
@@ -30859,7 +30853,7 @@
         <v>4429</v>
       </c>
       <c r="Z223" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="224" spans="1:26">
@@ -30936,7 +30930,7 @@
         <v>4429</v>
       </c>
       <c r="Z224" t="s">
-        <v>4450</v>
+        <v>4449</v>
       </c>
     </row>
     <row r="225" spans="1:26">
@@ -31164,7 +31158,7 @@
         <v>4429</v>
       </c>
       <c r="Z227" t="s">
-        <v>4456</v>
+        <v>4454</v>
       </c>
     </row>
     <row r="228" spans="1:26">
@@ -31466,7 +31460,7 @@
         <v>4429</v>
       </c>
       <c r="Z231" t="s">
-        <v>4456</v>
+        <v>4454</v>
       </c>
     </row>
     <row r="232" spans="1:26">
@@ -31614,7 +31608,7 @@
         <v>4429</v>
       </c>
       <c r="Z233" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="234" spans="1:26">
@@ -31691,7 +31685,7 @@
         <v>4429</v>
       </c>
       <c r="Z234" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="235" spans="1:26">
@@ -31765,7 +31759,7 @@
         <v>4429</v>
       </c>
       <c r="Z235" t="s">
-        <v>4456</v>
+        <v>4454</v>
       </c>
     </row>
     <row r="236" spans="1:26">
@@ -31839,7 +31833,7 @@
         <v>4429</v>
       </c>
       <c r="Z236" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="237" spans="1:26">
@@ -32064,7 +32058,7 @@
         <v>4429</v>
       </c>
       <c r="Z239" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="240" spans="1:26">
@@ -32141,7 +32135,7 @@
         <v>4429</v>
       </c>
       <c r="Z240" t="s">
-        <v>4447</v>
+        <v>4446</v>
       </c>
     </row>
     <row r="241" spans="1:26">
@@ -32218,7 +32212,7 @@
         <v>4429</v>
       </c>
       <c r="Z241" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="242" spans="1:26">
@@ -32366,7 +32360,7 @@
         <v>4429</v>
       </c>
       <c r="Z243" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="244" spans="1:26">
@@ -32440,7 +32434,7 @@
         <v>4429</v>
       </c>
       <c r="Z244" t="s">
-        <v>4456</v>
+        <v>4454</v>
       </c>
     </row>
     <row r="245" spans="1:26">
@@ -32591,7 +32585,7 @@
         <v>4429</v>
       </c>
       <c r="Z246" t="s">
-        <v>4447</v>
+        <v>4446</v>
       </c>
     </row>
     <row r="247" spans="1:26">
@@ -32739,7 +32733,7 @@
         <v>4429</v>
       </c>
       <c r="Z248" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="249" spans="1:26">
@@ -32893,7 +32887,7 @@
         <v>4429</v>
       </c>
       <c r="Z250" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="251" spans="1:26">
@@ -32967,7 +32961,7 @@
         <v>4429</v>
       </c>
       <c r="Z251" t="s">
-        <v>4451</v>
+        <v>4450</v>
       </c>
     </row>
     <row r="252" spans="1:26">
@@ -33044,7 +33038,7 @@
         <v>4429</v>
       </c>
       <c r="Z252" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="253" spans="1:26">
@@ -33121,7 +33115,7 @@
         <v>4429</v>
       </c>
       <c r="Z253" t="s">
-        <v>4456</v>
+        <v>4454</v>
       </c>
     </row>
     <row r="254" spans="1:26">
@@ -33198,7 +33192,7 @@
         <v>4429</v>
       </c>
       <c r="Z254" t="s">
-        <v>4452</v>
+        <v>4451</v>
       </c>
     </row>
     <row r="255" spans="1:26">
@@ -33349,7 +33343,7 @@
         <v>4429</v>
       </c>
       <c r="Z256" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="257" spans="1:26">
@@ -33580,7 +33574,7 @@
         <v>4429</v>
       </c>
       <c r="Z259" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="260" spans="1:26">
@@ -33814,7 +33808,7 @@
         <v>4429</v>
       </c>
       <c r="Z262" t="s">
-        <v>4450</v>
+        <v>4449</v>
       </c>
     </row>
     <row r="263" spans="1:26">
@@ -33968,7 +33962,7 @@
         <v>4429</v>
       </c>
       <c r="Z264" t="s">
-        <v>4447</v>
+        <v>4446</v>
       </c>
     </row>
     <row r="265" spans="1:26">
@@ -34199,7 +34193,7 @@
         <v>4429</v>
       </c>
       <c r="Z267" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="268" spans="1:26">
@@ -34273,7 +34267,7 @@
         <v>4429</v>
       </c>
       <c r="Z268" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="269" spans="1:26">
@@ -34578,7 +34572,7 @@
         <v>4431</v>
       </c>
       <c r="Z272" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="273" spans="1:26">
@@ -34806,7 +34800,7 @@
         <v>4432</v>
       </c>
       <c r="Z275" t="s">
-        <v>4456</v>
+        <v>4454</v>
       </c>
     </row>
     <row r="276" spans="1:26">
@@ -34883,7 +34877,7 @@
         <v>4432</v>
       </c>
       <c r="Z276" t="s">
-        <v>4456</v>
+        <v>4454</v>
       </c>
     </row>
     <row r="277" spans="1:26">
@@ -34957,7 +34951,7 @@
         <v>4432</v>
       </c>
       <c r="Z277" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="278" spans="1:26">
@@ -35185,7 +35179,7 @@
         <v>4432</v>
       </c>
       <c r="Z280" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="281" spans="1:26">
@@ -35339,7 +35333,7 @@
         <v>4432</v>
       </c>
       <c r="Z282" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="283" spans="1:26">
@@ -35413,7 +35407,7 @@
         <v>4432</v>
       </c>
       <c r="Z283" t="s">
-        <v>4448</v>
+        <v>4447</v>
       </c>
     </row>
     <row r="284" spans="1:26">
@@ -35487,7 +35481,7 @@
         <v>4432</v>
       </c>
       <c r="Z284" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="285" spans="1:26">
@@ -35638,7 +35632,7 @@
         <v>4432</v>
       </c>
       <c r="Z286" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="287" spans="1:26">
@@ -35712,7 +35706,7 @@
         <v>4432</v>
       </c>
       <c r="Z287" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="288" spans="1:26">
@@ -35934,7 +35928,7 @@
         <v>4432</v>
       </c>
       <c r="Z290" t="s">
-        <v>4456</v>
+        <v>4454</v>
       </c>
     </row>
     <row r="291" spans="1:26">
@@ -36008,7 +36002,7 @@
         <v>4432</v>
       </c>
       <c r="Z291" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="292" spans="1:26">
@@ -36085,7 +36079,7 @@
         <v>4432</v>
       </c>
       <c r="Z292" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="293" spans="1:26">
@@ -36159,7 +36153,7 @@
         <v>4432</v>
       </c>
       <c r="Z293" t="s">
-        <v>4456</v>
+        <v>4454</v>
       </c>
     </row>
     <row r="294" spans="1:26">
@@ -36233,7 +36227,7 @@
         <v>4432</v>
       </c>
       <c r="Z294" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="295" spans="1:26">
@@ -36307,7 +36301,7 @@
         <v>4432</v>
       </c>
       <c r="Z295" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="296" spans="1:26">
@@ -36381,7 +36375,7 @@
         <v>4431</v>
       </c>
       <c r="Z296" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="297" spans="1:26">
@@ -36532,7 +36526,7 @@
         <v>4431</v>
       </c>
       <c r="Z298" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="299" spans="1:26">
@@ -36683,7 +36677,7 @@
         <v>4431</v>
       </c>
       <c r="Z300" t="s">
-        <v>4450</v>
+        <v>4449</v>
       </c>
     </row>
     <row r="301" spans="1:26">
@@ -36757,7 +36751,7 @@
         <v>4431</v>
       </c>
       <c r="Z301" t="s">
-        <v>4446</v>
+        <v>4445</v>
       </c>
     </row>
     <row r="302" spans="1:26">
@@ -36831,7 +36825,7 @@
         <v>4431</v>
       </c>
       <c r="Z302" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="303" spans="1:26">
@@ -36985,7 +36979,7 @@
         <v>4431</v>
       </c>
       <c r="Z304" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="305" spans="1:26">
@@ -37059,7 +37053,7 @@
         <v>4431</v>
       </c>
       <c r="Z305" t="s">
-        <v>4447</v>
+        <v>4446</v>
       </c>
     </row>
     <row r="306" spans="1:26">
@@ -37133,7 +37127,7 @@
         <v>4431</v>
       </c>
       <c r="Z306" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="307" spans="1:26">
@@ -37210,7 +37204,7 @@
         <v>4431</v>
       </c>
       <c r="Z307" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="308" spans="1:26">
@@ -37364,7 +37358,7 @@
         <v>4431</v>
       </c>
       <c r="Z309" t="s">
-        <v>4450</v>
+        <v>4436</v>
       </c>
     </row>
     <row r="310" spans="1:26">
@@ -37441,7 +37435,7 @@
         <v>4431</v>
       </c>
       <c r="Z310" t="s">
-        <v>4453</v>
+        <v>4452</v>
       </c>
     </row>
     <row r="311" spans="1:26">
@@ -37518,7 +37512,7 @@
         <v>4431</v>
       </c>
       <c r="Z311" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="312" spans="1:26">
@@ -37595,7 +37589,7 @@
         <v>4431</v>
       </c>
       <c r="Z312" t="s">
-        <v>4456</v>
+        <v>4454</v>
       </c>
     </row>
     <row r="313" spans="1:26">
@@ -37746,7 +37740,7 @@
         <v>4431</v>
       </c>
       <c r="Z314" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="315" spans="1:26">
@@ -37897,7 +37891,7 @@
         <v>4430</v>
       </c>
       <c r="Z316" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="317" spans="1:26">
@@ -38051,7 +38045,7 @@
         <v>4430</v>
       </c>
       <c r="Z318" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="319" spans="1:26">
@@ -38125,7 +38119,7 @@
         <v>4430</v>
       </c>
       <c r="Z319" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="320" spans="1:26">
@@ -38276,7 +38270,7 @@
         <v>4430</v>
       </c>
       <c r="Z321" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="322" spans="1:26">
@@ -38350,7 +38344,7 @@
         <v>4430</v>
       </c>
       <c r="Z322" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="323" spans="1:26">
@@ -38427,7 +38421,7 @@
         <v>4430</v>
       </c>
       <c r="Z323" t="s">
-        <v>4455</v>
+        <v>4453</v>
       </c>
     </row>
     <row r="324" spans="1:26">
@@ -38732,7 +38726,7 @@
         <v>4430</v>
       </c>
       <c r="Z327" t="s">
-        <v>4454</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="328" spans="1:26">
@@ -38809,7 +38803,7 @@
         <v>4430</v>
       </c>
       <c r="Z328" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="329" spans="1:26">
@@ -38960,7 +38954,7 @@
         <v>4430</v>
       </c>
       <c r="Z330" t="s">
-        <v>4457</v>
+        <v>4455</v>
       </c>
     </row>
     <row r="331" spans="1:26">
@@ -39037,7 +39031,7 @@
         <v>4430</v>
       </c>
       <c r="Z331" t="s">
-        <v>4456</v>
+        <v>4454</v>
       </c>
     </row>
     <row r="332" spans="1:26">
@@ -39111,7 +39105,7 @@
         <v>4430</v>
       </c>
       <c r="Z332" t="s">
-        <v>4456</v>
+        <v>4454</v>
       </c>
     </row>
     <row r="333" spans="1:26">
@@ -39342,7 +39336,7 @@
         <v>4430</v>
       </c>
       <c r="Z335" t="s">
-        <v>4456</v>
+        <v>4454</v>
       </c>
     </row>
     <row r="336" spans="1:26">
@@ -39496,7 +39490,7 @@
         <v>4430</v>
       </c>
       <c r="Z337" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="338" spans="1:26">
@@ -39650,7 +39644,7 @@
         <v>4430</v>
       </c>
       <c r="Z339" t="s">
-        <v>4456</v>
+        <v>4454</v>
       </c>
     </row>
     <row r="340" spans="1:26">
@@ -39724,7 +39718,7 @@
         <v>4430</v>
       </c>
       <c r="Z340" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="341" spans="1:26">
@@ -39798,7 +39792,7 @@
         <v>4430</v>
       </c>
       <c r="Z341" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="342" spans="1:26">
@@ -39872,7 +39866,7 @@
         <v>4430</v>
       </c>
       <c r="Z342" t="s">
-        <v>4456</v>
+        <v>4454</v>
       </c>
     </row>
     <row r="343" spans="1:26">
@@ -39946,7 +39940,7 @@
         <v>4430</v>
       </c>
       <c r="Z343" t="s">
-        <v>4446</v>
+        <v>4445</v>
       </c>
     </row>
     <row r="344" spans="1:26">
@@ -40020,7 +40014,7 @@
         <v>4430</v>
       </c>
       <c r="Z344" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="345" spans="1:26">
@@ -40171,7 +40165,7 @@
         <v>4430</v>
       </c>
       <c r="Z346" t="s">
-        <v>4457</v>
+        <v>4455</v>
       </c>
     </row>
     <row r="347" spans="1:26">
@@ -40245,7 +40239,7 @@
         <v>4430</v>
       </c>
       <c r="Z347" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="348" spans="1:26">
@@ -40322,7 +40316,7 @@
         <v>4430</v>
       </c>
       <c r="Z348" t="s">
-        <v>4447</v>
+        <v>4446</v>
       </c>
     </row>
     <row r="349" spans="1:26">
@@ -40544,7 +40538,7 @@
         <v>4432</v>
       </c>
       <c r="Z351" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="352" spans="1:26">
@@ -40621,7 +40615,7 @@
         <v>4432</v>
       </c>
       <c r="Z352" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="353" spans="1:26">
@@ -40695,7 +40689,7 @@
         <v>4432</v>
       </c>
       <c r="Z353" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="354" spans="1:26">
@@ -40846,7 +40840,7 @@
         <v>4432</v>
       </c>
       <c r="Z355" t="s">
-        <v>4450</v>
+        <v>4449</v>
       </c>
     </row>
     <row r="356" spans="1:26">
@@ -40997,7 +40991,7 @@
         <v>4432</v>
       </c>
       <c r="Z357" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="358" spans="1:26">
@@ -41071,7 +41065,7 @@
         <v>4432</v>
       </c>
       <c r="Z358" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="359" spans="1:26">
@@ -41145,7 +41139,7 @@
         <v>4432</v>
       </c>
       <c r="Z359" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="360" spans="1:26">
@@ -41219,7 +41213,7 @@
         <v>4432</v>
       </c>
       <c r="Z360" t="s">
-        <v>4455</v>
+        <v>4453</v>
       </c>
     </row>
     <row r="361" spans="1:26">
@@ -41293,7 +41287,7 @@
         <v>4432</v>
       </c>
       <c r="Z361" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="362" spans="1:26">
@@ -41370,7 +41364,7 @@
         <v>4432</v>
       </c>
       <c r="Z362" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="363" spans="1:26">
@@ -41444,7 +41438,7 @@
         <v>4432</v>
       </c>
       <c r="Z363" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="364" spans="1:26">
@@ -41900,7 +41894,7 @@
         <v>4432</v>
       </c>
       <c r="Z369" t="s">
-        <v>4456</v>
+        <v>4454</v>
       </c>
     </row>
     <row r="370" spans="1:26">
@@ -41974,7 +41968,7 @@
         <v>4432</v>
       </c>
       <c r="Z370" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="371" spans="1:26">
@@ -42273,7 +42267,7 @@
         <v>4432</v>
       </c>
       <c r="Z374" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="375" spans="1:26">
@@ -42427,7 +42421,7 @@
         <v>4432</v>
       </c>
       <c r="Z376" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="377" spans="1:26">
@@ -42578,7 +42572,7 @@
         <v>4432</v>
       </c>
       <c r="Z378" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="379" spans="1:26">
@@ -42655,7 +42649,7 @@
         <v>4432</v>
       </c>
       <c r="Z379" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="380" spans="1:26">
@@ -42732,7 +42726,7 @@
         <v>4432</v>
       </c>
       <c r="Z380" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="381" spans="1:26">
@@ -42806,7 +42800,7 @@
         <v>4432</v>
       </c>
       <c r="Z381" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="382" spans="1:26">
@@ -42883,7 +42877,7 @@
         <v>4432</v>
       </c>
       <c r="Z382" t="s">
-        <v>4447</v>
+        <v>4446</v>
       </c>
     </row>
     <row r="383" spans="1:26">
@@ -42960,7 +42954,7 @@
         <v>4432</v>
       </c>
       <c r="Z383" t="s">
-        <v>4447</v>
+        <v>4446</v>
       </c>
     </row>
     <row r="384" spans="1:26">
@@ -43111,7 +43105,7 @@
         <v>4432</v>
       </c>
       <c r="Z385" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="386" spans="1:26">
@@ -43188,7 +43182,7 @@
         <v>4432</v>
       </c>
       <c r="Z386" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="387" spans="1:26">
@@ -43265,7 +43259,7 @@
         <v>4432</v>
       </c>
       <c r="Z387" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="388" spans="1:26">
@@ -43570,7 +43564,7 @@
         <v>4432</v>
       </c>
       <c r="Z391" t="s">
-        <v>4448</v>
+        <v>4447</v>
       </c>
     </row>
     <row r="392" spans="1:26">
@@ -43647,7 +43641,7 @@
         <v>4432</v>
       </c>
       <c r="Z392" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="393" spans="1:26">
@@ -43798,7 +43792,7 @@
         <v>4432</v>
       </c>
       <c r="Z394" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="395" spans="1:26">
@@ -43875,7 +43869,7 @@
         <v>4432</v>
       </c>
       <c r="Z395" t="s">
-        <v>4447</v>
+        <v>4446</v>
       </c>
     </row>
     <row r="396" spans="1:26">
@@ -43949,7 +43943,7 @@
         <v>4432</v>
       </c>
       <c r="Z396" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="397" spans="1:26">
@@ -44100,7 +44094,7 @@
         <v>4432</v>
       </c>
       <c r="Z398" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="399" spans="1:26">
@@ -44174,7 +44168,7 @@
         <v>4432</v>
       </c>
       <c r="Z399" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="400" spans="1:26">
@@ -44325,7 +44319,7 @@
         <v>4432</v>
       </c>
       <c r="Z401" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="402" spans="1:26">
@@ -44399,7 +44393,7 @@
         <v>4432</v>
       </c>
       <c r="Z402" t="s">
-        <v>4455</v>
+        <v>4453</v>
       </c>
     </row>
     <row r="403" spans="1:26">
@@ -44461,7 +44455,7 @@
         <v>4432</v>
       </c>
       <c r="Z403" t="s">
-        <v>4457</v>
+        <v>4455</v>
       </c>
     </row>
     <row r="404" spans="1:26">
@@ -44612,7 +44606,7 @@
         <v>4432</v>
       </c>
       <c r="Z405" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="406" spans="1:26">
@@ -44689,7 +44683,7 @@
         <v>4432</v>
       </c>
       <c r="Z406" t="s">
-        <v>4455</v>
+        <v>4453</v>
       </c>
     </row>
     <row r="407" spans="1:26">
@@ -44843,7 +44837,7 @@
         <v>4432</v>
       </c>
       <c r="Z408" t="s">
-        <v>4455</v>
+        <v>4453</v>
       </c>
     </row>
     <row r="409" spans="1:26">
@@ -44994,7 +44988,7 @@
         <v>4432</v>
       </c>
       <c r="Z410" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="411" spans="1:26">
@@ -45071,7 +45065,7 @@
         <v>4432</v>
       </c>
       <c r="Z411" t="s">
-        <v>4450</v>
+        <v>4449</v>
       </c>
     </row>
     <row r="412" spans="1:26">
@@ -45148,7 +45142,7 @@
         <v>4429</v>
       </c>
       <c r="Z412" t="s">
-        <v>4450</v>
+        <v>4449</v>
       </c>
     </row>
     <row r="413" spans="1:26">
@@ -45225,7 +45219,7 @@
         <v>4429</v>
       </c>
       <c r="Z413" t="s">
-        <v>4448</v>
+        <v>4447</v>
       </c>
     </row>
     <row r="414" spans="1:26">
@@ -45453,7 +45447,7 @@
         <v>4429</v>
       </c>
       <c r="Z416" t="s">
-        <v>4455</v>
+        <v>4453</v>
       </c>
     </row>
     <row r="417" spans="1:26">
@@ -45530,7 +45524,7 @@
         <v>4429</v>
       </c>
       <c r="Z417" t="s">
-        <v>4457</v>
+        <v>4455</v>
       </c>
     </row>
     <row r="418" spans="1:26">
@@ -45607,7 +45601,7 @@
         <v>4429</v>
       </c>
       <c r="Z418" t="s">
-        <v>4444</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="419" spans="1:26">
@@ -45684,7 +45678,7 @@
         <v>4429</v>
       </c>
       <c r="Z419" t="s">
-        <v>4447</v>
+        <v>4446</v>
       </c>
     </row>
     <row r="420" spans="1:26">
@@ -45758,7 +45752,7 @@
         <v>4429</v>
       </c>
       <c r="Z420" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="421" spans="1:26">
@@ -45983,7 +45977,7 @@
         <v>4429</v>
       </c>
       <c r="Z423" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="424" spans="1:26">
@@ -46134,7 +46128,7 @@
         <v>4429</v>
       </c>
       <c r="Z425" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="426" spans="1:26">
@@ -46211,7 +46205,7 @@
         <v>4429</v>
       </c>
       <c r="Z426" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="427" spans="1:26">
@@ -46436,7 +46430,7 @@
         <v>4429</v>
       </c>
       <c r="Z429" t="s">
-        <v>4447</v>
+        <v>4446</v>
       </c>
     </row>
     <row r="430" spans="1:26">
@@ -46587,7 +46581,7 @@
         <v>4429</v>
       </c>
       <c r="Z431" t="s">
-        <v>4455</v>
+        <v>4453</v>
       </c>
     </row>
     <row r="432" spans="1:26">
@@ -46892,7 +46886,7 @@
         <v>4431</v>
       </c>
       <c r="Z435" t="s">
-        <v>4454</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="436" spans="1:26">
@@ -47046,7 +47040,7 @@
         <v>4433</v>
       </c>
       <c r="Z437" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="438" spans="1:26">
@@ -47123,7 +47117,7 @@
         <v>4433</v>
       </c>
       <c r="Z438" t="s">
-        <v>4450</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="439" spans="1:26">
@@ -47197,7 +47191,7 @@
         <v>4433</v>
       </c>
       <c r="Z439" t="s">
-        <v>4450</v>
+        <v>4449</v>
       </c>
     </row>
     <row r="440" spans="1:26">
@@ -47428,7 +47422,7 @@
         <v>4433</v>
       </c>
       <c r="Z442" t="s">
-        <v>4456</v>
+        <v>4454</v>
       </c>
     </row>
     <row r="443" spans="1:26">
@@ -47502,7 +47496,7 @@
         <v>4433</v>
       </c>
       <c r="Z443" t="s">
-        <v>4451</v>
+        <v>4450</v>
       </c>
     </row>
     <row r="444" spans="1:26">
@@ -47576,7 +47570,7 @@
         <v>4433</v>
       </c>
       <c r="Z444" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="445" spans="1:26">
@@ -47653,7 +47647,7 @@
         <v>4433</v>
       </c>
       <c r="Z445" t="s">
-        <v>4457</v>
+        <v>4455</v>
       </c>
     </row>
     <row r="446" spans="1:26">
@@ -47727,7 +47721,7 @@
         <v>4433</v>
       </c>
       <c r="Z446" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="447" spans="1:26">
@@ -47804,7 +47798,7 @@
         <v>4433</v>
       </c>
       <c r="Z447" t="s">
-        <v>4451</v>
+        <v>4450</v>
       </c>
     </row>
     <row r="448" spans="1:26">
@@ -47955,7 +47949,7 @@
         <v>4433</v>
       </c>
       <c r="Z449" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="450" spans="1:26">
@@ -48032,7 +48026,7 @@
         <v>4433</v>
       </c>
       <c r="Z450" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="451" spans="1:26">
@@ -48334,7 +48328,7 @@
         <v>4433</v>
       </c>
       <c r="Z454" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="455" spans="1:26">
@@ -48408,7 +48402,7 @@
         <v>4433</v>
       </c>
       <c r="Z455" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="456" spans="1:26">
@@ -48482,7 +48476,7 @@
         <v>4433</v>
       </c>
       <c r="Z456" t="s">
-        <v>4453</v>
+        <v>4452</v>
       </c>
     </row>
     <row r="457" spans="1:26">
@@ -48633,7 +48627,7 @@
         <v>4433</v>
       </c>
       <c r="Z458" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="459" spans="1:26">
@@ -48929,7 +48923,7 @@
         <v>4433</v>
       </c>
       <c r="Z462" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="463" spans="1:26">
@@ -49077,7 +49071,7 @@
         <v>4433</v>
       </c>
       <c r="Z464" t="s">
-        <v>4456</v>
+        <v>4454</v>
       </c>
     </row>
     <row r="465" spans="1:26">
@@ -49154,7 +49148,7 @@
         <v>4433</v>
       </c>
       <c r="Z465" t="s">
-        <v>4450</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="466" spans="1:26">
@@ -49231,7 +49225,7 @@
         <v>4433</v>
       </c>
       <c r="Z466" t="s">
-        <v>4456</v>
+        <v>4454</v>
       </c>
     </row>
     <row r="467" spans="1:26">
@@ -49382,7 +49376,7 @@
         <v>4433</v>
       </c>
       <c r="Z468" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="469" spans="1:26">
@@ -49610,7 +49604,7 @@
         <v>4433</v>
       </c>
       <c r="Z471" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="472" spans="1:26">
@@ -49761,7 +49755,7 @@
         <v>4431</v>
       </c>
       <c r="Z473" t="s">
-        <v>4448</v>
+        <v>4447</v>
       </c>
     </row>
     <row r="474" spans="1:26">
@@ -49989,7 +49983,7 @@
         <v>4431</v>
       </c>
       <c r="Z476" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="477" spans="1:26">
@@ -50140,7 +50134,7 @@
         <v>4431</v>
       </c>
       <c r="Z478" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="479" spans="1:26">
@@ -50217,7 +50211,7 @@
         <v>4431</v>
       </c>
       <c r="Z479" t="s">
-        <v>4444</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="480" spans="1:26">
@@ -50294,7 +50288,7 @@
         <v>4431</v>
       </c>
       <c r="Z480" t="s">
-        <v>4450</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="481" spans="1:26">
@@ -50371,7 +50365,7 @@
         <v>4431</v>
       </c>
       <c r="Z481" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="482" spans="1:26">
@@ -50445,7 +50439,7 @@
         <v>4431</v>
       </c>
       <c r="Z482" t="s">
-        <v>4447</v>
+        <v>4446</v>
       </c>
     </row>
     <row r="483" spans="1:26">
@@ -50522,7 +50516,7 @@
         <v>4431</v>
       </c>
       <c r="Z483" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="484" spans="1:26">
@@ -50596,7 +50590,7 @@
         <v>4431</v>
       </c>
       <c r="Z484" t="s">
-        <v>4453</v>
+        <v>4452</v>
       </c>
     </row>
     <row r="485" spans="1:26">
@@ -50673,7 +50667,7 @@
         <v>4431</v>
       </c>
       <c r="Z485" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="486" spans="1:26">
@@ -50827,7 +50821,7 @@
         <v>4431</v>
       </c>
       <c r="Z487" t="s">
-        <v>4454</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="488" spans="1:26">
@@ -50978,7 +50972,7 @@
         <v>4431</v>
       </c>
       <c r="Z489" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="490" spans="1:26">
@@ -51055,7 +51049,7 @@
         <v>4431</v>
       </c>
       <c r="Z490" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="491" spans="1:26">
@@ -51206,7 +51200,7 @@
         <v>4431</v>
       </c>
       <c r="Z492" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="493" spans="1:26">
@@ -51280,7 +51274,7 @@
         <v>4431</v>
       </c>
       <c r="Z493" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="494" spans="1:26">
@@ -51508,7 +51502,7 @@
         <v>4431</v>
       </c>
       <c r="Z496" t="s">
-        <v>4456</v>
+        <v>4454</v>
       </c>
     </row>
     <row r="497" spans="1:26">
@@ -51582,7 +51576,7 @@
         <v>4431</v>
       </c>
       <c r="Z497" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="498" spans="1:26">
@@ -51807,7 +51801,7 @@
         <v>4431</v>
       </c>
       <c r="Z500" t="s">
-        <v>4453</v>
+        <v>4452</v>
       </c>
     </row>
     <row r="501" spans="1:26">
@@ -51881,7 +51875,7 @@
         <v>4431</v>
       </c>
       <c r="Z501" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="502" spans="1:26">
@@ -51955,7 +51949,7 @@
         <v>4431</v>
       </c>
       <c r="Z502" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="503" spans="1:26">
@@ -52106,7 +52100,7 @@
         <v>4431</v>
       </c>
       <c r="Z504" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="505" spans="1:26">
@@ -52180,7 +52174,7 @@
         <v>4431</v>
       </c>
       <c r="Z505" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="506" spans="1:26">
@@ -52257,7 +52251,7 @@
         <v>4431</v>
       </c>
       <c r="Z506" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="507" spans="1:26">
@@ -52331,7 +52325,7 @@
         <v>4431</v>
       </c>
       <c r="Z507" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="508" spans="1:26">
@@ -52408,7 +52402,7 @@
         <v>4431</v>
       </c>
       <c r="Z508" t="s">
-        <v>4444</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="509" spans="1:26">
@@ -52485,7 +52479,7 @@
         <v>4431</v>
       </c>
       <c r="Z509" t="s">
-        <v>4450</v>
+        <v>4449</v>
       </c>
     </row>
     <row r="510" spans="1:26">
@@ -52559,7 +52553,7 @@
         <v>4431</v>
       </c>
       <c r="Z510" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="511" spans="1:26">
@@ -52636,7 +52630,7 @@
         <v>4431</v>
       </c>
       <c r="Z511" t="s">
-        <v>4451</v>
+        <v>4450</v>
       </c>
     </row>
     <row r="512" spans="1:26">
@@ -52713,7 +52707,7 @@
         <v>4431</v>
       </c>
       <c r="Z512" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="513" spans="1:26">
@@ -52787,7 +52781,7 @@
         <v>4431</v>
       </c>
       <c r="Z513" t="s">
-        <v>4451</v>
+        <v>4450</v>
       </c>
     </row>
     <row r="514" spans="1:26">
@@ -53012,7 +53006,7 @@
         <v>4431</v>
       </c>
       <c r="Z516" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="517" spans="1:26">
@@ -53086,7 +53080,7 @@
         <v>4431</v>
       </c>
       <c r="Z517" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="518" spans="1:26">
@@ -53237,7 +53231,7 @@
         <v>4429</v>
       </c>
       <c r="Z519" t="s">
-        <v>4448</v>
+        <v>4447</v>
       </c>
     </row>
     <row r="520" spans="1:26">
@@ -53314,7 +53308,7 @@
         <v>4429</v>
       </c>
       <c r="Z520" t="s">
-        <v>4450</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="521" spans="1:26">
@@ -53545,7 +53539,7 @@
         <v>4429</v>
       </c>
       <c r="Z523" t="s">
-        <v>4450</v>
+        <v>4449</v>
       </c>
     </row>
     <row r="524" spans="1:26">
@@ -53622,7 +53616,7 @@
         <v>4429</v>
       </c>
       <c r="Z524" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="525" spans="1:26">
@@ -53699,7 +53693,7 @@
         <v>4429</v>
       </c>
       <c r="Z525" t="s">
-        <v>4456</v>
+        <v>4454</v>
       </c>
     </row>
     <row r="526" spans="1:26">
@@ -53773,7 +53767,7 @@
         <v>4429</v>
       </c>
       <c r="Z526" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="527" spans="1:26">
@@ -53850,7 +53844,7 @@
         <v>4429</v>
       </c>
       <c r="Z527" t="s">
-        <v>4448</v>
+        <v>4447</v>
       </c>
     </row>
     <row r="528" spans="1:26">
@@ -54229,7 +54223,7 @@
         <v>1927</v>
       </c>
       <c r="Z532" t="s">
-        <v>4450</v>
+        <v>4449</v>
       </c>
     </row>
     <row r="533" spans="1:26">
@@ -54383,7 +54377,7 @@
         <v>1927</v>
       </c>
       <c r="Z534" t="s">
-        <v>4447</v>
+        <v>4446</v>
       </c>
     </row>
     <row r="535" spans="1:26">
@@ -54457,7 +54451,7 @@
         <v>1927</v>
       </c>
       <c r="Z535" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="536" spans="1:26">
@@ -54762,7 +54756,7 @@
         <v>1927</v>
       </c>
       <c r="Z539" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="540" spans="1:26">
@@ -54916,7 +54910,7 @@
         <v>1927</v>
       </c>
       <c r="Z541" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="542" spans="1:26">
@@ -54993,7 +54987,7 @@
         <v>1927</v>
       </c>
       <c r="Z542" t="s">
-        <v>4450</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="543" spans="1:26">
@@ -55144,7 +55138,7 @@
         <v>1927</v>
       </c>
       <c r="Z544" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="545" spans="1:26">
@@ -55529,7 +55523,7 @@
         <v>4433</v>
       </c>
       <c r="Z549" t="s">
-        <v>4451</v>
+        <v>4450</v>
       </c>
     </row>
     <row r="550" spans="1:26">
@@ -55603,7 +55597,7 @@
         <v>4433</v>
       </c>
       <c r="Z550" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="551" spans="1:26">
@@ -55754,7 +55748,7 @@
         <v>4430</v>
       </c>
       <c r="Z552" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="553" spans="1:26">
@@ -56130,7 +56124,7 @@
         <v>4430</v>
       </c>
       <c r="Z557" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="558" spans="1:26">
@@ -56361,7 +56355,7 @@
         <v>4430</v>
       </c>
       <c r="Z560" t="s">
-        <v>4451</v>
+        <v>4450</v>
       </c>
     </row>
     <row r="561" spans="1:26">
@@ -56438,7 +56432,7 @@
         <v>4430</v>
       </c>
       <c r="Z561" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="562" spans="1:26">
@@ -56512,7 +56506,7 @@
         <v>4430</v>
       </c>
       <c r="Z562" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="563" spans="1:26">
@@ -56586,7 +56580,7 @@
         <v>4430</v>
       </c>
       <c r="Z563" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="564" spans="1:26">
@@ -56737,7 +56731,7 @@
         <v>4430</v>
       </c>
       <c r="Z565" t="s">
-        <v>4456</v>
+        <v>4454</v>
       </c>
     </row>
     <row r="566" spans="1:26">
@@ -56811,7 +56805,7 @@
         <v>4430</v>
       </c>
       <c r="Z566" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="567" spans="1:26">
@@ -57042,7 +57036,7 @@
         <v>4430</v>
       </c>
       <c r="Z569" t="s">
-        <v>4450</v>
+        <v>4436</v>
       </c>
     </row>
     <row r="570" spans="1:26">
@@ -57116,7 +57110,7 @@
         <v>4430</v>
       </c>
       <c r="Z570" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="571" spans="1:26">
@@ -57190,7 +57184,7 @@
         <v>4430</v>
       </c>
       <c r="Z571" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="572" spans="1:26">
@@ -57338,7 +57332,7 @@
         <v>4430</v>
       </c>
       <c r="Z573" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="574" spans="1:26">
@@ -57415,7 +57409,7 @@
         <v>4430</v>
       </c>
       <c r="Z574" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="575" spans="1:26">
@@ -57489,7 +57483,7 @@
         <v>4430</v>
       </c>
       <c r="Z575" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="576" spans="1:26">
@@ -57640,7 +57634,7 @@
         <v>4430</v>
       </c>
       <c r="Z577" t="s">
-        <v>4447</v>
+        <v>4446</v>
       </c>
     </row>
     <row r="578" spans="1:26">
@@ -57714,7 +57708,7 @@
         <v>4430</v>
       </c>
       <c r="Z578" t="s">
-        <v>4448</v>
+        <v>4447</v>
       </c>
     </row>
     <row r="579" spans="1:26">
@@ -57865,7 +57859,7 @@
         <v>4429</v>
       </c>
       <c r="Z580" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="581" spans="1:26">
@@ -58019,7 +58013,7 @@
         <v>4429</v>
       </c>
       <c r="Z582" t="s">
-        <v>4454</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="583" spans="1:26">
@@ -58170,7 +58164,7 @@
         <v>4429</v>
       </c>
       <c r="Z584" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="585" spans="1:26">
@@ -58244,7 +58238,7 @@
         <v>4429</v>
       </c>
       <c r="Z585" t="s">
-        <v>4447</v>
+        <v>4446</v>
       </c>
     </row>
     <row r="586" spans="1:26">
@@ -58321,7 +58315,7 @@
         <v>4429</v>
       </c>
       <c r="Z586" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="587" spans="1:26">
@@ -58697,7 +58691,7 @@
         <v>4429</v>
       </c>
       <c r="Z591" t="s">
-        <v>4456</v>
+        <v>4454</v>
       </c>
     </row>
     <row r="592" spans="1:26">
@@ -58774,7 +58768,7 @@
         <v>4429</v>
       </c>
       <c r="Z592" t="s">
-        <v>4447</v>
+        <v>4446</v>
       </c>
     </row>
     <row r="593" spans="1:26">
@@ -58925,7 +58919,7 @@
         <v>4429</v>
       </c>
       <c r="Z594" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="595" spans="1:26">
@@ -58999,7 +58993,7 @@
         <v>4429</v>
       </c>
       <c r="Z595" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="596" spans="1:26">
@@ -59076,7 +59070,7 @@
         <v>4429</v>
       </c>
       <c r="Z596" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="597" spans="1:26">
@@ -59150,7 +59144,7 @@
         <v>4429</v>
       </c>
       <c r="Z597" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="598" spans="1:26">
@@ -59227,7 +59221,7 @@
         <v>4430</v>
       </c>
       <c r="Z598" t="s">
-        <v>4452</v>
+        <v>4451</v>
       </c>
     </row>
     <row r="599" spans="1:26">
@@ -59304,7 +59298,7 @@
         <v>4430</v>
       </c>
       <c r="Z599" t="s">
-        <v>4450</v>
+        <v>4449</v>
       </c>
     </row>
     <row r="600" spans="1:26">
@@ -59381,7 +59375,7 @@
         <v>4430</v>
       </c>
       <c r="Z600" t="s">
-        <v>4454</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="601" spans="1:26">
@@ -59455,7 +59449,7 @@
         <v>4430</v>
       </c>
       <c r="Z601" t="s">
-        <v>4451</v>
+        <v>4450</v>
       </c>
     </row>
     <row r="602" spans="1:26">
@@ -59529,7 +59523,7 @@
         <v>4430</v>
       </c>
       <c r="Z602" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="603" spans="1:26">
@@ -59831,7 +59825,7 @@
         <v>4432</v>
       </c>
       <c r="Z606" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="607" spans="1:26">
@@ -59908,7 +59902,7 @@
         <v>4432</v>
       </c>
       <c r="Z607" t="s">
-        <v>4451</v>
+        <v>4450</v>
       </c>
     </row>
     <row r="608" spans="1:26">
@@ -59985,7 +59979,7 @@
         <v>4432</v>
       </c>
       <c r="Z608" t="s">
-        <v>4447</v>
+        <v>4446</v>
       </c>
     </row>
     <row r="609" spans="1:26">
@@ -60136,7 +60130,7 @@
         <v>4432</v>
       </c>
       <c r="Z610" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="611" spans="1:26">
@@ -60213,7 +60207,7 @@
         <v>4431</v>
       </c>
       <c r="Z611" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="612" spans="1:26">
@@ -60515,7 +60509,7 @@
         <v>4431</v>
       </c>
       <c r="Z615" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="616" spans="1:26">
@@ -60592,7 +60586,7 @@
         <v>4431</v>
       </c>
       <c r="Z616" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="617" spans="1:26">
@@ -60746,7 +60740,7 @@
         <v>4433</v>
       </c>
       <c r="Z618" t="s">
-        <v>4453</v>
+        <v>4452</v>
       </c>
     </row>
     <row r="619" spans="1:26">
@@ -60820,7 +60814,7 @@
         <v>4433</v>
       </c>
       <c r="Z619" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="620" spans="1:26">
@@ -60894,7 +60888,7 @@
         <v>4433</v>
       </c>
       <c r="Z620" t="s">
-        <v>4450</v>
+        <v>4449</v>
       </c>
     </row>
     <row r="621" spans="1:26">
@@ -61045,7 +61039,7 @@
         <v>4433</v>
       </c>
       <c r="Z622" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="623" spans="1:26">
@@ -61122,7 +61116,7 @@
         <v>4433</v>
       </c>
       <c r="Z623" t="s">
-        <v>4456</v>
+        <v>4454</v>
       </c>
     </row>
     <row r="624" spans="1:26">
@@ -61196,7 +61190,7 @@
         <v>4433</v>
       </c>
       <c r="Z624" t="s">
-        <v>4456</v>
+        <v>4454</v>
       </c>
     </row>
     <row r="625" spans="1:26">
@@ -61347,7 +61341,7 @@
         <v>4433</v>
       </c>
       <c r="Z626" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="627" spans="1:26">
@@ -61424,7 +61418,7 @@
         <v>4431</v>
       </c>
       <c r="Z627" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="628" spans="1:26">
@@ -61578,7 +61572,7 @@
         <v>4431</v>
       </c>
       <c r="Z629" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="630" spans="1:26">
@@ -61655,7 +61649,7 @@
         <v>4431</v>
       </c>
       <c r="Z630" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="631" spans="1:26">
@@ -61883,7 +61877,7 @@
         <v>4431</v>
       </c>
       <c r="Z633" t="s">
-        <v>4448</v>
+        <v>4447</v>
       </c>
     </row>
     <row r="634" spans="1:26">
@@ -62188,7 +62182,7 @@
         <v>4433</v>
       </c>
       <c r="Z637" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="638" spans="1:26">
@@ -62342,7 +62336,7 @@
         <v>4433</v>
       </c>
       <c r="Z639" t="s">
-        <v>4447</v>
+        <v>4446</v>
       </c>
     </row>
     <row r="640" spans="1:26">
@@ -62419,7 +62413,7 @@
         <v>4430</v>
       </c>
       <c r="Z640" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="641" spans="1:26">
@@ -62727,7 +62721,7 @@
         <v>4433</v>
       </c>
       <c r="Z644" t="s">
-        <v>4447</v>
+        <v>4446</v>
       </c>
     </row>
     <row r="645" spans="1:26">
@@ -62801,7 +62795,7 @@
         <v>4433</v>
       </c>
       <c r="Z645" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="646" spans="1:26">
@@ -62878,7 +62872,7 @@
         <v>4433</v>
       </c>
       <c r="Z646" t="s">
-        <v>4455</v>
+        <v>4453</v>
       </c>
     </row>
     <row r="647" spans="1:26">
@@ -62955,7 +62949,7 @@
         <v>4433</v>
       </c>
       <c r="Z647" t="s">
-        <v>4457</v>
+        <v>4455</v>
       </c>
     </row>
     <row r="648" spans="1:26">
@@ -63032,7 +63026,7 @@
         <v>4433</v>
       </c>
       <c r="Z648" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="649" spans="1:26">
@@ -63106,7 +63100,7 @@
         <v>4433</v>
       </c>
       <c r="Z649" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="650" spans="1:26">
@@ -63260,7 +63254,7 @@
         <v>4433</v>
       </c>
       <c r="Z651" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="652" spans="1:26">
@@ -63337,7 +63331,7 @@
         <v>4433</v>
       </c>
       <c r="Z652" t="s">
-        <v>4452</v>
+        <v>4451</v>
       </c>
     </row>
     <row r="653" spans="1:26">
@@ -63414,7 +63408,7 @@
         <v>4433</v>
       </c>
       <c r="Z653" t="s">
-        <v>4455</v>
+        <v>4453</v>
       </c>
     </row>
     <row r="654" spans="1:26">
@@ -63488,7 +63482,7 @@
         <v>4433</v>
       </c>
       <c r="Z654" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="655" spans="1:26">
@@ -63562,7 +63556,7 @@
         <v>4433</v>
       </c>
       <c r="Z655" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="656" spans="1:26">
@@ -63710,7 +63704,7 @@
         <v>4433</v>
       </c>
       <c r="Z657" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="658" spans="1:26">
@@ -63784,7 +63778,7 @@
         <v>4433</v>
       </c>
       <c r="Z658" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="659" spans="1:26">
@@ -63858,7 +63852,7 @@
         <v>4434</v>
       </c>
       <c r="Z659" t="s">
-        <v>4448</v>
+        <v>4447</v>
       </c>
     </row>
     <row r="660" spans="1:26">
@@ -64012,7 +64006,7 @@
         <v>4431</v>
       </c>
       <c r="Z661" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="662" spans="1:26">
@@ -64089,7 +64083,7 @@
         <v>4431</v>
       </c>
       <c r="Z662" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="663" spans="1:26">
@@ -64243,7 +64237,7 @@
         <v>4431</v>
       </c>
       <c r="Z664" t="s">
-        <v>4450</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="665" spans="1:26">
@@ -64320,7 +64314,7 @@
         <v>4432</v>
       </c>
       <c r="Z665" t="s">
-        <v>4455</v>
+        <v>4453</v>
       </c>
     </row>
     <row r="666" spans="1:26">
@@ -64471,7 +64465,7 @@
         <v>4432</v>
       </c>
       <c r="Z667" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="668" spans="1:26">
@@ -64545,7 +64539,7 @@
         <v>4432</v>
       </c>
       <c r="Z668" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="669" spans="1:26">
@@ -64619,7 +64613,7 @@
         <v>4432</v>
       </c>
       <c r="Z669" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="670" spans="1:26">
@@ -64693,7 +64687,7 @@
         <v>4435</v>
       </c>
       <c r="Z670" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="671" spans="1:26">
@@ -64767,7 +64761,7 @@
         <v>4435</v>
       </c>
       <c r="Z671" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="672" spans="1:26">
@@ -64844,7 +64838,7 @@
         <v>4435</v>
       </c>
       <c r="Z672" t="s">
-        <v>4448</v>
+        <v>4447</v>
       </c>
     </row>
     <row r="673" spans="1:26">
@@ -64921,7 +64915,7 @@
         <v>4435</v>
       </c>
       <c r="Z673" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="674" spans="1:26">
@@ -65069,7 +65063,7 @@
         <v>4435</v>
       </c>
       <c r="Z675" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="676" spans="1:26">
@@ -65220,7 +65214,7 @@
         <v>4435</v>
       </c>
       <c r="Z677" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="678" spans="1:26">
@@ -65371,7 +65365,7 @@
         <v>4432</v>
       </c>
       <c r="Z679" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="680" spans="1:26">
@@ -65445,7 +65439,7 @@
         <v>4433</v>
       </c>
       <c r="Z680" t="s">
-        <v>4456</v>
+        <v>4454</v>
       </c>
     </row>
     <row r="681" spans="1:26">
@@ -65519,7 +65513,7 @@
         <v>4433</v>
       </c>
       <c r="Z681" t="s">
-        <v>4456</v>
+        <v>4454</v>
       </c>
     </row>
     <row r="682" spans="1:26">
@@ -65593,7 +65587,7 @@
         <v>4433</v>
       </c>
       <c r="Z682" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="683" spans="1:26">
@@ -66049,7 +66043,7 @@
         <v>4433</v>
       </c>
       <c r="Z688" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="689" spans="1:26">
@@ -66123,7 +66117,7 @@
         <v>4433</v>
       </c>
       <c r="Z689" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="690" spans="1:26">
@@ -66200,7 +66194,7 @@
         <v>4433</v>
       </c>
       <c r="Z690" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="691" spans="1:26">
@@ -66354,7 +66348,7 @@
         <v>4433</v>
       </c>
       <c r="Z692" t="s">
-        <v>4447</v>
+        <v>4446</v>
       </c>
     </row>
     <row r="693" spans="1:26">
@@ -66502,7 +66496,7 @@
         <v>4433</v>
       </c>
       <c r="Z694" t="s">
-        <v>4456</v>
+        <v>4454</v>
       </c>
     </row>
     <row r="695" spans="1:26">
@@ -66576,7 +66570,7 @@
         <v>4433</v>
       </c>
       <c r="Z695" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="696" spans="1:26">
@@ -66730,7 +66724,7 @@
         <v>4430</v>
       </c>
       <c r="Z697" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="698" spans="1:26">
@@ -67032,7 +67026,7 @@
         <v>4430</v>
       </c>
       <c r="Z701" t="s">
-        <v>4444</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="702" spans="1:26">
@@ -67109,7 +67103,7 @@
         <v>4430</v>
       </c>
       <c r="Z702" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="703" spans="1:26">
@@ -67183,7 +67177,7 @@
         <v>4430</v>
       </c>
       <c r="Z703" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="704" spans="1:26">
@@ -67642,7 +67636,7 @@
         <v>4429</v>
       </c>
       <c r="Z709" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="710" spans="1:26">
@@ -67796,7 +67790,7 @@
         <v>4429</v>
       </c>
       <c r="Z711" t="s">
-        <v>4454</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="712" spans="1:26">
@@ -68095,7 +68089,7 @@
         <v>4433</v>
       </c>
       <c r="Z715" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="716" spans="1:26">
@@ -68169,7 +68163,7 @@
         <v>4433</v>
       </c>
       <c r="Z716" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="717" spans="1:26">
@@ -68243,7 +68237,7 @@
         <v>4433</v>
       </c>
       <c r="Z717" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="718" spans="1:26">
@@ -68542,7 +68536,7 @@
         <v>4433</v>
       </c>
       <c r="Z721" t="s">
-        <v>4456</v>
+        <v>4454</v>
       </c>
     </row>
     <row r="722" spans="1:26">
@@ -68773,7 +68767,7 @@
         <v>4431</v>
       </c>
       <c r="Z724" t="s">
-        <v>4454</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="725" spans="1:26">
@@ -68847,7 +68841,7 @@
         <v>4431</v>
       </c>
       <c r="Z725" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="726" spans="1:26">
@@ -69149,7 +69143,7 @@
         <v>4432</v>
       </c>
       <c r="Z729" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="730" spans="1:26">
@@ -69303,7 +69297,7 @@
         <v>4432</v>
       </c>
       <c r="Z731" t="s">
-        <v>4446</v>
+        <v>4445</v>
       </c>
     </row>
     <row r="732" spans="1:26">
@@ -69377,7 +69371,7 @@
         <v>4432</v>
       </c>
       <c r="Z732" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="733" spans="1:26">
@@ -69451,7 +69445,7 @@
         <v>4432</v>
       </c>
       <c r="Z733" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="734" spans="1:26">
@@ -69525,7 +69519,7 @@
         <v>4432</v>
       </c>
       <c r="Z734" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="735" spans="1:26">
@@ -69676,7 +69670,7 @@
         <v>4432</v>
       </c>
       <c r="Z736" t="s">
-        <v>4436</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="737" spans="1:26">
@@ -69753,7 +69747,7 @@
         <v>4434</v>
       </c>
       <c r="Z737" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
   </sheetData>

</xml_diff>